<commit_message>
Updated with table edits
</commit_message>
<xml_diff>
--- a/parameters/invtmt_portfolio_mapper.xlsx
+++ b/parameters/invtmt_portfolio_mapper.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
   <si>
     <t>Security Name</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Diff in holdings?</t>
   </si>
   <si>
-    <t>Notes for reconcilliation</t>
-  </si>
-  <si>
     <t>Holdings</t>
   </si>
   <si>
@@ -209,13 +206,25 @@
     <t>Exchange Rate @</t>
   </si>
   <si>
-    <t>PRICE_OBTAINED_FROM</t>
-  </si>
-  <si>
-    <t>BID_PRICE_OBTAINED_FROM</t>
-  </si>
-  <si>
-    <t>ASK_PRICE_OBTAINED_FROM</t>
+    <t>REFIN</t>
+  </si>
+  <si>
+    <t>HOLDINGSPERCONFIRMATION</t>
+  </si>
+  <si>
+    <t>CUSTODIANCONFIDENCELEVEL</t>
+  </si>
+  <si>
+    <t>PRICE</t>
+  </si>
+  <si>
+    <t>BIDPRICE</t>
+  </si>
+  <si>
+    <t>ASKPRICE</t>
+  </si>
+  <si>
+    <t>Notes for reconciliation</t>
   </si>
 </sst>
 </file>
@@ -444,6 +453,7 @@
       <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
@@ -453,7 +463,6 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -736,25 +745,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="58" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
         <v>57</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -762,7 +771,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -770,7 +779,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -778,7 +787,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -786,7 +795,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -794,7 +803,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -802,7 +811,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -810,7 +819,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -818,20 +827,24 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="5" t="s">
@@ -841,189 +854,191 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="3"/>
+        <v>66</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>61</v>
+        <v>19</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>63</v>
       </c>
       <c r="C20" s="3"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" s="3"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>62</v>
+        <v>31</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>64</v>
       </c>
       <c r="C27" s="7"/>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>63</v>
+        <v>32</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>65</v>
       </c>
       <c r="C28" s="7"/>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C32" s="9"/>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="9"/>
+    </row>
+    <row r="34" spans="1:3" ht="28.5">
+      <c r="A34" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C33" s="9"/>
-    </row>
-    <row r="34" spans="1:3" ht="28.5">
-      <c r="A34" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C34" s="10" t="s">
+    </row>
+    <row r="35" spans="1:3" ht="140.5">
+      <c r="A35" s="15"/>
+      <c r="C35" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="140.5">
-      <c r="A35" s="14"/>
-      <c r="C35" s="10" t="s">
+    <row r="36" spans="1:3" ht="112.5">
+      <c r="A36" s="16"/>
+      <c r="C36" s="10" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="112.5">
-      <c r="A36" s="15"/>
-      <c r="C36" s="10" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1031,8 +1046,9 @@
     <mergeCell ref="A34:A36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <customProperties>
-    <customPr name="OrphanNamesChecked" r:id="rId1"/>
+    <customPr name="OrphanNamesChecked" r:id="rId2"/>
   </customProperties>
 </worksheet>
 </file>
</xml_diff>